<commit_message>
alter the filter options
</commit_message>
<xml_diff>
--- a/static/requred_files/sample_student_data.xlsx
+++ b/static/requred_files/sample_student_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cgpa_track-master\static\requred_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,9 +47,6 @@
     <t>bag_of_log</t>
   </si>
   <si>
-    <t>no_of_arrear</t>
-  </si>
-  <si>
     <t>semester1</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>reg_no</t>
+  </si>
+  <si>
+    <t>history_of_arrear</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -466,31 +466,31 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update in excel file
</commit_message>
<xml_diff>
--- a/static/requred_files/sample_student_data.xlsx
+++ b/static/requred_files/sample_student_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>batch</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>history_of_arrear</t>
+  </si>
+  <si>
+    <t>diploma</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,19 +431,19 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -463,37 +466,40 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -511,8 +517,9 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -530,8 +537,9 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
   </sheetData>

</xml_diff>